<commit_message>
24ene2017 started to work again
</commit_message>
<xml_diff>
--- a/result1.xlsx
+++ b/result1.xlsx
@@ -1286,11 +1286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="314031968"/>
-        <c:axId val="314033600"/>
+        <c:axId val="-97492224"/>
+        <c:axId val="-97480256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="314031968"/>
+        <c:axId val="-97492224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314033600"/>
+        <c:crossAx val="-97480256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314033600"/>
+        <c:axId val="-97480256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314031968"/>
+        <c:crossAx val="-97492224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2252,11 +2252,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="314037952"/>
-        <c:axId val="314025984"/>
+        <c:axId val="-97482976"/>
+        <c:axId val="-97477536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="314037952"/>
+        <c:axId val="-97482976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314025984"/>
+        <c:crossAx val="-97477536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2362,7 +2362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314025984"/>
+        <c:axId val="-97477536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2468,7 +2468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314037952"/>
+        <c:crossAx val="-97482976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>